<commit_message>
⚡️ Fixed ACO and added instances
</commit_message>
<xml_diff>
--- a/A2/Knapsack Instances/Known Optimums.xlsx
+++ b/A2/Knapsack Instances/Known Optimums.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6095e57c740b7128/Tayla Uni/Computer Science/COS 314 S1/Assignments/A2/Knapsack Instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_1E09BD0997E904C9EC7FC3C64D0F582CE8D30305" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{663D2CC4-FA45-461E-ACC4-106654DB1E89}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_E876579872CA18C8EC7FC3C64D013869816A0C98" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C34B69B-84F0-48D1-9BB9-A49FA2FAC46D}"/>
   <bookViews>
-    <workbookView xWindow="31215" yWindow="2400" windowWidth="17250" windowHeight="9405" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,12 +86,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -474,7 +476,7 @@
         <v>295</v>
       </c>
       <c r="C2" t="str">
-        <f>_xlfn.CONCAT(A2, " ", B2)</f>
+        <f>_xlfn.CONCAT(A2," ",B2)</f>
         <v>f1_l-d_kp_10_269 295</v>
       </c>
     </row>
@@ -486,7 +488,7 @@
         <v>1024</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C12" si="0">_xlfn.CONCAT(A3, " ", B3)</f>
+        <f t="shared" ref="C3:C12" si="0">_xlfn.CONCAT(A3," ",B3)</f>
         <v>f2_l-d_kp_20_878 1024</v>
       </c>
     </row>

</xml_diff>